<commit_message>
Improved example feature names
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/SphinxFeatureMap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="15132" windowHeight="9240" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="15132" windowHeight="9240"/>
   </bookViews>
   <sheets>
     <sheet name="Container Features" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="128">
   <si>
     <t>Eclipse Platform Extensions</t>
   </si>
@@ -363,40 +363,22 @@
     <t>Compare Team Support (Subversive SVN)</t>
   </si>
   <si>
-    <t>UML2 IDE Integration</t>
-  </si>
-  <si>
     <t>Exemplary UML2 IDE integration including Model Explorer view contribution for UML2 content, and generic UML2 form editor</t>
   </si>
   <si>
     <t>IDE integration of EMF Extended Library example  including Model Explorer view contribution for Extended Library content, and generic Extended Library form editor</t>
   </si>
   <si>
-    <t>Extended Library IDE integration</t>
-  </si>
-  <si>
-    <t>Navigator Examples</t>
-  </si>
-  <si>
-    <t>Hummingbird Metamodels and IDE Integration</t>
-  </si>
-  <si>
     <t>Hummingbird metamodels and IDE integration including Model Explorer view contribution for Hummingbird content, generic Hummingbird form editor, exemplary graphical Hummingbird editors, exemplary validation services and constraints for Hummingbird, exemplary compare &amp; merge support for Hummingbird, model transformation and code generation examples for Hummingbird, and more</t>
   </si>
   <si>
     <t>Exemplary Xtend/Xpand IDE integration including model transformation and code generation context menu contributions, preferences for Xpand outlets, and more</t>
   </si>
   <si>
-    <t>Validation IDE Integration</t>
-  </si>
-  <si>
     <t>Examplary Validation IDE integration including context menu contributions and actions for invoking validation in various ways</t>
   </si>
   <si>
     <t>Generic Model Explorer view</t>
-  </si>
-  <si>
-    <t>Core Examples</t>
   </si>
   <si>
     <t>Includes Sphinx Perspective, exemplary generic model manipulation actions, and more</t>
@@ -435,6 +417,51 @@
   </si>
   <si>
     <t>Common logic for Common Navigator views that operate on Sphinx-managed shared model instances and integrate into the load/edit/save lifecycle of the same</t>
+  </si>
+  <si>
+    <t>Sphinx Xtend/Xpand IDE Integration</t>
+  </si>
+  <si>
+    <t>Sphinx Compare Team Support (Subversive SVN)</t>
+  </si>
+  <si>
+    <t>Sphinx Compare Engine &amp; Editor</t>
+  </si>
+  <si>
+    <t>Sphinx Validation Runtime Extensions</t>
+  </si>
+  <si>
+    <t>Sphinx Graphiti Editor Sockets</t>
+  </si>
+  <si>
+    <t>Sphinx GMF Editor Sockets</t>
+  </si>
+  <si>
+    <t>Sphinx Form Editor Sockets</t>
+  </si>
+  <si>
+    <t>Sphinx Common Navigator Sockets</t>
+  </si>
+  <si>
+    <t>Sphinx Core Examples</t>
+  </si>
+  <si>
+    <t>Sphinx Navigator Examples</t>
+  </si>
+  <si>
+    <t>Sphinx Exemplary Validation IDE Integration</t>
+  </si>
+  <si>
+    <t>Sphinx Exemplary Xtend/Xpand IDE Integration</t>
+  </si>
+  <si>
+    <t>Sphinx Hummingbird Metamodels and IDE Integration Examples</t>
+  </si>
+  <si>
+    <t>Sphinx Exemplary UML2 IDE Integration</t>
+  </si>
+  <si>
+    <t>Sphinx Exemplary Extended Library IDE integration</t>
   </si>
 </sst>
 </file>
@@ -584,7 +611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -667,21 +694,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -691,10 +703,19 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1012,9 +1033,7 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1054,7 +1073,7 @@
         <v>76</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="12" t="s">
@@ -1068,10 +1087,10 @@
       <c r="A3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="31" t="s">
         <v>84</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1088,10 +1107,10 @@
       <c r="A4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="31" t="s">
         <v>85</v>
       </c>
       <c r="D4" s="24" t="s">
@@ -1142,10 +1161,10 @@
       <c r="A7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="31" t="s">
         <v>87</v>
       </c>
       <c r="D7" s="21" t="s">
@@ -1209,8 +1228,8 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1248,21 +1267,20 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="32" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="25" t="str">
-        <f>B2</f>
-        <v>Common Navigator Sockets</v>
+      <c r="D2" s="29" t="s">
+        <v>120</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F2" s="25" t="s">
         <v>26</v>
@@ -1270,19 +1288,18 @@
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="37" t="s">
+      <c r="A3" s="37"/>
+      <c r="B3" s="32" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="25" t="str">
-        <f>B3</f>
-        <v>Form Editor Sockets</v>
+      <c r="D3" s="29" t="s">
+        <v>119</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>12</v>
@@ -1290,19 +1307,18 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="37" t="s">
+      <c r="A4" s="37"/>
+      <c r="B4" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="25" t="str">
-        <f>B4</f>
-        <v>GMF Editor Sockets</v>
+      <c r="D4" s="29" t="s">
+        <v>118</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F4" s="29" t="s">
         <v>43</v>
@@ -1310,19 +1326,18 @@
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="25" t="str">
-        <f>B5</f>
-        <v>Graphiti Editor Sockets</v>
+      <c r="D5" s="29" t="s">
+        <v>117</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>29</v>
@@ -1337,12 +1352,11 @@
       <c r="C6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="25" t="str">
-        <f>A6</f>
-        <v>Validation Runtime Extensions</v>
+      <c r="D6" s="29" t="s">
+        <v>116</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F6" s="29" t="s">
         <v>25</v>
@@ -1350,7 +1364,7 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="37" t="s">
         <v>91</v>
       </c>
       <c r="B7" s="19" t="s">
@@ -1359,12 +1373,11 @@
       <c r="C7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="25" t="str">
-        <f>B7</f>
-        <v>Compare Engine &amp; Editor</v>
+      <c r="D7" s="29" t="s">
+        <v>115</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>27</v>
@@ -1372,19 +1385,18 @@
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="37" t="s">
+      <c r="A8" s="37"/>
+      <c r="B8" s="32" t="s">
         <v>94</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="25" t="str">
-        <f>B8</f>
-        <v>Compare Team Support (Subversive SVN)</v>
+      <c r="D8" s="29" t="s">
+        <v>114</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F8" s="25" t="s">
         <v>28</v>
@@ -1395,18 +1407,17 @@
       <c r="A9" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="32" t="s">
         <v>93</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="25" t="str">
-        <f>B9</f>
-        <v>Xtend/Xpand IDE Integration</v>
+      <c r="D9" s="29" t="s">
+        <v>113</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>30</v>
@@ -1414,51 +1425,51 @@
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="40" t="s">
-        <v>114</v>
+      <c r="D10" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>108</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="30"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="41"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="31"/>
+      <c r="G11" s="34"/>
     </row>
     <row r="12" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="42"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="35"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" s="4"/>
@@ -1487,14 +1498,14 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1" outlineLevel="1"/>
     <col min="3" max="3" width="43" style="1" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="61.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" customWidth="1"/>
@@ -1520,10 +1531,10 @@
         <v>51</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>52</v>
@@ -1534,10 +1545,10 @@
         <v>49</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>46</v>
@@ -1548,10 +1559,10 @@
         <v>48</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>50</v>
@@ -1562,10 +1573,10 @@
         <v>47</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>45</v>
@@ -1576,10 +1587,10 @@
         <v>54</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>53</v>
@@ -1590,10 +1601,10 @@
         <v>56</v>
       </c>
       <c r="B7" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>95</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>96</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>58</v>
@@ -1604,10 +1615,10 @@
         <v>57</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Improved container source feature names and descriptions
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/SphinxFeatureMap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="127">
   <si>
     <t>Eclipse Platform Extensions</t>
   </si>
@@ -312,9 +312,6 @@
     <t>Sphinx Documentation</t>
   </si>
   <si>
-    <t>Sphinx Sources</t>
-  </si>
-  <si>
     <t>Sphinx SDK</t>
   </si>
   <si>
@@ -330,15 +327,9 @@
     <t>Third-Party Components for Sphinx</t>
   </si>
   <si>
-    <t>Includes source code for Sphinx runtime binaries</t>
-  </si>
-  <si>
     <t>Includes Sphinx Developer Guide (Help)</t>
   </si>
   <si>
-    <t>Includes Sphinx examples (with sources)</t>
-  </si>
-  <si>
     <t>Includes Sphinx unit and integration tests</t>
   </si>
   <si>
@@ -346,9 +337,6 @@
   </si>
   <si>
     <t>Includes third-party components required by Sphinx (selected Orbit plug-ins)</t>
-  </si>
-  <si>
-    <t>Includes Sphinx runtime, sources and documentation (but no examples)</t>
   </si>
   <si>
     <t>Compare &amp; Merge IDE Integration</t>
@@ -410,9 +398,6 @@
     <t>Subversive-based support for using Sphinx-based compare and merge editors in team operations with SVN repositories</t>
   </si>
   <si>
-    <t>Includes Sphinx runtime binaries (without sources and documentation)</t>
-  </si>
-  <si>
     <t>Sphinx Core</t>
   </si>
   <si>
@@ -462,6 +447,18 @@
   </si>
   <si>
     <t>Sphinx Exemplary Extended Library IDE integration</t>
+  </si>
+  <si>
+    <t>Includes Sphinx runtime binaries (without source code and documentation)</t>
+  </si>
+  <si>
+    <t>Includes Sphinx runtime, source code and documentation (but no examples)</t>
+  </si>
+  <si>
+    <t>Includes Sphinx examples (with source code)</t>
+  </si>
+  <si>
+    <t>automatically generated</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1030,9 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1073,7 +1072,7 @@
         <v>76</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="12" t="s">
@@ -1083,15 +1082,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>78</v>
+        <v>126</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>84</v>
+        <v>126</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>65</v>
@@ -1111,7 +1110,7 @@
         <v>77</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>61</v>
@@ -1126,10 +1125,10 @@
         <v>32</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="12" t="s">
@@ -1144,10 +1143,10 @@
         <v>33</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
@@ -1162,10 +1161,10 @@
         <v>38</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>44</v>
@@ -1182,10 +1181,10 @@
         <v>34</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>37</v>
@@ -1200,10 +1199,10 @@
         <v>35</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>36</v>
@@ -1229,7 +1228,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1277,10 +1276,10 @@
         <v>15</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F2" s="25" t="s">
         <v>26</v>
@@ -1296,10 +1295,10 @@
         <v>12</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>12</v>
@@ -1315,10 +1314,10 @@
         <v>13</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F4" s="29" t="s">
         <v>43</v>
@@ -1334,10 +1333,10 @@
         <v>14</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>29</v>
@@ -1353,10 +1352,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F6" s="29" t="s">
         <v>25</v>
@@ -1365,7 +1364,7 @@
     </row>
     <row r="7" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>59</v>
@@ -1374,10 +1373,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>27</v>
@@ -1387,16 +1386,16 @@
     <row r="8" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
       <c r="B8" s="32" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F8" s="25" t="s">
         <v>28</v>
@@ -1405,19 +1404,19 @@
     </row>
     <row r="9" spans="1:7" ht="66" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>30</v>
@@ -1435,10 +1434,10 @@
         <v>6</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>24</v>
@@ -1531,10 +1530,10 @@
         <v>51</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>52</v>
@@ -1545,10 +1544,10 @@
         <v>49</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>46</v>
@@ -1559,10 +1558,10 @@
         <v>48</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>50</v>
@@ -1573,10 +1572,10 @@
         <v>47</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>45</v>
@@ -1587,10 +1586,10 @@
         <v>54</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>53</v>
@@ -1601,10 +1600,10 @@
         <v>56</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>58</v>
@@ -1615,10 +1614,10 @@
         <v>57</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Improved container feature descriptions
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/SphinxFeatureMap.xlsx
@@ -333,9 +333,6 @@
     <t>Includes Sphinx unit and integration tests</t>
   </si>
   <si>
-    <t>Includes utilities for JUnit-based Sphinx integration tests running against a predefined reference workspace (with sources)</t>
-  </si>
-  <si>
     <t>Includes third-party components required by Sphinx (selected Orbit plug-ins)</t>
   </si>
   <si>
@@ -459,6 +456,9 @@
   </si>
   <si>
     <t>automatically generated</t>
+  </si>
+  <si>
+    <t>Includes utilities for JUnit-based Sphinx integration tests running against a predefined reference workspace (with source code)</t>
   </si>
 </sst>
 </file>
@@ -1030,8 +1030,8 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1072,7 +1072,7 @@
         <v>76</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="12" t="s">
@@ -1087,10 +1087,10 @@
         <v>60</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>65</v>
@@ -1128,7 +1128,7 @@
         <v>78</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="12" t="s">
@@ -1146,7 +1146,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
@@ -1184,7 +1184,7 @@
         <v>81</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>37</v>
@@ -1202,7 +1202,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>36</v>
@@ -1276,10 +1276,10 @@
         <v>15</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" s="25" t="s">
         <v>26</v>
@@ -1295,10 +1295,10 @@
         <v>12</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>12</v>
@@ -1314,10 +1314,10 @@
         <v>13</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" s="29" t="s">
         <v>43</v>
@@ -1333,10 +1333,10 @@
         <v>14</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>29</v>
@@ -1352,10 +1352,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" s="29" t="s">
         <v>25</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="7" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>59</v>
@@ -1373,10 +1373,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>27</v>
@@ -1386,16 +1386,16 @@
     <row r="8" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
       <c r="B8" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F8" s="25" t="s">
         <v>28</v>
@@ -1404,19 +1404,19 @@
     </row>
     <row r="9" spans="1:7" ht="66" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="32" t="s">
         <v>88</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>89</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>30</v>
@@ -1434,10 +1434,10 @@
         <v>6</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>24</v>
@@ -1530,10 +1530,10 @@
         <v>51</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>52</v>
@@ -1544,10 +1544,10 @@
         <v>49</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>46</v>
@@ -1558,10 +1558,10 @@
         <v>48</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>50</v>
@@ -1572,10 +1572,10 @@
         <v>47</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>45</v>
@@ -1586,10 +1586,10 @@
         <v>54</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>53</v>
@@ -1600,10 +1600,10 @@
         <v>56</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>58</v>
@@ -1614,10 +1614,10 @@
         <v>57</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
RESOLVED bug - 393840: [Examples] Provide example illustrating implementation of validation constraints for Sphinx-enabled metamodel https://bugs.eclipse.org/bugs/show_bug.cgi?id=393840
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/SphinxFeatureMap.xlsx
@@ -747,7 +747,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -760,9 +760,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -800,7 +800,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -872,7 +872,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1536,7 +1536,7 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated Sphinx feature map
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/SphinxFeatureMap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="15132" windowHeight="9240" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="15132" windowHeight="9240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Container Features" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="132">
   <si>
     <t>Eclipse Platform Extensions</t>
   </si>
@@ -424,17 +424,6 @@
   </si>
   <si>
     <t>Includes utilities for JUnit-based Sphinx integration tests running against a predefined reference workspace (with source code)</t>
-  </si>
-  <si>
-    <t>org.eclipse.sphinx.emf.navigators
-org.eclipse.sphinx.emf.editors.forms org.eclipse.sphinx.emf.editors.forms.nebula 
-org.eclipse.sphinx.gmf.editors
-org.eclipse.sphinx.graphiti.editors
-org.eclipse.sphinx.emf.validation
-org.eclipse.sphinx.emf.compare
-org.eclipse.sphinx.emf.compare.team.subversive
-org.eclipse.sphinx.xtendxpand
-org.eclipse.sphinx.core</t>
   </si>
   <si>
     <t>org.eclipse.sphinx.examples.core
@@ -468,6 +457,23 @@
 org.eclipse.sphinx.examples.hummingbird20.codegen.xpand.newwizard
 org.eclipse.sphinx.examples.hummingbird20.transform.xtend.newwizard
 org.eclipse.sphinx.examples.sampleworkspace.newwizard</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.emf.navigators
+org.eclipse.sphinx.emf.editors.forms org.eclipse.sphinx.emf.editors.forms.nebula 
+org.eclipse.sphinx.gmf.editors
+org.eclipse.sphinx.graphiti.editors
+org.eclipse.sphinx.emf.validation
+org.eclipse.sphinx.emf.compare
+org.eclipse.sphinx.emf.compare.team.subversive
+org.eclipse.sphinx.xtendxpand     org.eclipse.sphinx.pde
+org.eclipse.sphinx.core</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.pde</t>
+  </si>
+  <si>
+    <t>Sphinx PDE</t>
   </si>
 </sst>
 </file>
@@ -617,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -718,12 +724,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -733,6 +733,24 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -747,7 +765,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -760,9 +778,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -800,7 +818,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -872,7 +890,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1051,8 +1069,8 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1103,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="132" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
@@ -1097,7 +1115,7 @@
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="34" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>39</v>
@@ -1171,7 +1189,7 @@
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>39</v>
@@ -1246,10 +1264,10 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1287,7 +1305,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="43" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="32" t="s">
@@ -1308,8 +1326,8 @@
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="43" t="s">
+      <c r="A3" s="43"/>
+      <c r="B3" s="47" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="33" t="s">
@@ -1327,24 +1345,24 @@
       <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="44"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="E4" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="E4" s="29" t="s">
-        <v>128</v>
-      </c>
       <c r="F4" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="32" t="s">
         <v>18</v>
       </c>
@@ -1363,7 +1381,7 @@
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="19" t="s">
         <v>19</v>
       </c>
@@ -1401,7 +1419,7 @@
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="43" t="s">
         <v>83</v>
       </c>
       <c r="B8" s="19" t="s">
@@ -1422,7 +1440,7 @@
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="32" t="s">
         <v>86</v>
       </c>
@@ -1461,65 +1479,82 @@
       </c>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="37"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G11" s="35"/>
+    </row>
+    <row r="12" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B12" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C12" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D12" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E12" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="35"/>
-    </row>
-    <row r="12" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="19" t="s">
+      <c r="G12" s="39"/>
+    </row>
+    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="43"/>
+      <c r="B13" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="9" t="s">
+      <c r="C13" s="42"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="36"/>
-    </row>
-    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="19" t="s">
+      <c r="G13" s="40"/>
+    </row>
+    <row r="14" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="43"/>
+      <c r="B14" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="9" t="s">
+      <c r="C14" s="42"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="37"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="4"/>
+      <c r="G14" s="41"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="C12:C14"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="D12:D14"/>
     <mergeCell ref="B3:B4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1536,7 +1571,7 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1631,7 +1666,7 @@
         <v>89</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
RESOLVED - bug 392464: [Navigator & Editor Sockets] Finish up Sphinx editor socket for GMF-based graphical editors https://bugs.eclipse.org/bugs/show_bug.cgi?id=392464
Added org.eclipse.sphinx.examples.hummingbird20.diagram.gmf example
plug-in
</commit_message>
<xml_diff>
--- a/docs/org.eclipse.sphinx.doc.design/SphinxFeatureMap.xlsx
+++ b/docs/org.eclipse.sphinx.doc.design/SphinxFeatureMap.xlsx
@@ -265,21 +265,6 @@
     <t>Sphinx Nebula Extensions for Form Editors</t>
   </si>
   <si>
-    <t>org.eclipse.sphinx.examples.hummingbird10
-org.eclipse.sphinx.examples.hummingbird10.edit
-org.eclipse.sphinx.examples.hummingbird10.editor
-org.eclipse.sphinx.examples.hummingbird20
-org.eclipse.sphinx.examples.hummingbird20.edit
-org.eclipse.sphinx.examples.hummingbird20.editor org.eclipse.sphinx.examples.hummingbird20.editors.nebula
-org.eclipse.sphinx.examples.hummingbird.ide
-org.eclipse.sphinx.examples.hummingbird.ide.ui
-org.eclipse.sphinx.examples.hummingbird.compare
-org.eclipse.sphinx.examples.hummingbird20.diagram.graphiti
-org.eclipse.sphinx.examples.hummingbird20.codegen.xpand.newwizard
-org.eclipse.sphinx.examples.hummingbird20.transform.xtend.newwizard
-org.eclipse.sphinx.examples.sampleworkspace.newwizard</t>
-  </si>
-  <si>
     <t>org.eclipse.sphinx.pde</t>
   </si>
   <si>
@@ -425,6 +410,21 @@
 org.eclipse.sphinx.emf.ui
 org.eclipse.sphinx.platform
 org.eclipse.sphinx.platform.ui</t>
+  </si>
+  <si>
+    <t>org.eclipse.sphinx.examples.hummingbird.ide
+org.eclipse.sphinx.examples.hummingbird.ide.ui
+org.eclipse.sphinx.examples.hummingbird10
+org.eclipse.sphinx.examples.hummingbird10.edit
+org.eclipse.sphinx.examples.hummingbird10.ide.ui
+org.eclipse.sphinx.examples.hummingbird20
+org.eclipse.sphinx.examples.hummingbird20.codegen.xpand.newwizard
+org.eclipse.sphinx.examples.hummingbird20.diagram.gmf
+org.eclipse.sphinx.examples.hummingbird20.edit
+org.eclipse.sphinx.examples.hummingbird20.editors.nebula
+org.eclipse.sphinx.examples.hummingbird20.ide.ui
+org.eclipse.sphinx.examples.hummingbird20.transform.xtend.newwizard
+org.eclipse.sphinx.examples.hummingbird20.validation</t>
   </si>
 </sst>
 </file>
@@ -592,13 +592,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:F11" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:F11" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A1:F11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="21" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Name" dataDxfId="20" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Description" dataDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Included plug-ins" dataDxfId="18" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Id" dataDxfId="19" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Name" dataDxfId="18" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Description" dataDxfId="17" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Included plug-ins" dataDxfId="16" dataCellStyle="Normal"/>
     <tableColumn id="5" name="Included features" dataDxfId="15" dataCellStyle="Normal"/>
     <tableColumn id="6" name="Update site/p2 repository category" dataDxfId="14" dataCellStyle="Normal"/>
   </tableColumns>
@@ -607,28 +607,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:F9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:F9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Top-level service" dataDxfId="13"/>
-    <tableColumn id="2" name="Sub services" dataDxfId="12"/>
-    <tableColumn id="3" name="Feature id" dataDxfId="11"/>
-    <tableColumn id="4" name="Feature name" dataDxfId="10"/>
-    <tableColumn id="5" name="Feature description" dataDxfId="9"/>
-    <tableColumn id="6" name="Included Plug-ins" dataDxfId="8"/>
+    <tableColumn id="1" name="Top-level service" dataDxfId="11"/>
+    <tableColumn id="2" name="Sub services" dataDxfId="10"/>
+    <tableColumn id="3" name="Feature id" dataDxfId="9"/>
+    <tableColumn id="4" name="Feature name" dataDxfId="8"/>
+    <tableColumn id="5" name="Feature description" dataDxfId="7"/>
+    <tableColumn id="6" name="Included Plug-ins" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A1:D8" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A1:D8" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D8"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Id" dataDxfId="5"/>
-    <tableColumn id="2" name="Name" dataDxfId="4"/>
-    <tableColumn id="3" name="Description" dataDxfId="3"/>
-    <tableColumn id="4" name="Included Plug-ins" dataDxfId="2"/>
+    <tableColumn id="1" name="Id" dataDxfId="3"/>
+    <tableColumn id="2" name="Name" dataDxfId="2"/>
+    <tableColumn id="3" name="Description" dataDxfId="1"/>
+    <tableColumn id="4" name="Included Plug-ins" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -958,7 +958,7 @@
         <v>43</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -969,13 +969,13 @@
         <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -983,16 +983,16 @@
         <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
@@ -1021,62 +1021,62 @@
         <v>51</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1087,13 +1087,13 @@
         <v>52</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>71</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1104,14 +1104,14 @@
         <v>53</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
@@ -1122,14 +1122,14 @@
         <v>54</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1170,7 +1170,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>46</v>
@@ -1199,7 +1199,7 @@
         <v>63</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>15</v>
@@ -1216,7 +1216,7 @@
         <v>62</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>7</v>
@@ -1230,7 +1230,7 @@
         <v>73</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>72</v>
@@ -1247,10 +1247,10 @@
         <v>61</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
@@ -1264,7 +1264,7 @@
         <v>60</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>14</v>
@@ -1284,7 +1284,7 @@
         <v>59</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>16</v>
@@ -1292,16 +1292,16 @@
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1309,7 +1309,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>3</v>
@@ -1318,10 +1318,10 @@
         <v>58</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1346,7 +1346,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1381,7 +1381,7 @@
         <v>64</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>32</v>
@@ -1395,7 +1395,7 @@
         <v>66</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>26</v>
@@ -1409,7 +1409,7 @@
         <v>67</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>30</v>
@@ -1423,13 +1423,13 @@
         <v>65</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -1437,10 +1437,10 @@
         <v>68</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
@@ -1451,7 +1451,7 @@
         <v>69</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>37</v>
@@ -1465,7 +1465,7 @@
         <v>70</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>34</v>

</xml_diff>